<commit_message>
Add missing results - Pete Lee and Peter andersson
</commit_message>
<xml_diff>
--- a/data/2020-12-08/SCW Weekly Comp 2020-12-08 (Responses).xlsx
+++ b/data/2020-12-08/SCW Weekly Comp 2020-12-08 (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-12-08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248D8914-5CFB-4B11-A8F2-804404E6E627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9D851-E7F8-4A2C-A57E-033B03741D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="227">
   <si>
     <t>Timestamp</t>
   </si>
@@ -689,6 +689,21 @@
   </si>
   <si>
     <t>1:43.76</t>
+  </si>
+  <si>
+    <t>12/15/2020 19:04:21</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/672444916797296?post_id=672985756743212&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>12/15/2020 20:11:55</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1026387727837469/?post_id=1029478957528346&amp;view=permalink&amp;__cft__[0]=AZXj2U_KvS9ECavsicJ2QyUQQNeQLZCEfAxZqQ2IdscdkkcrlBiqMHiL1jf4AFfZzaXEqS_6gRy03fBEGTb5mxPmalUnU0PL7vTnFR7AdvByWLhZMm_j67ReyiQt44y1l0k&amp;__tn__=%2CO%2CP-R</t>
+  </si>
+  <si>
+    <t>12:35.15</t>
   </si>
 </sst>
 </file>
@@ -698,7 +713,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -708,16 +723,32 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -734,7 +765,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -742,11 +773,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -754,8 +801,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="47" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -972,11 +1032,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CY60"/>
+  <dimension ref="A1:DE62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CI1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="CQ61" sqref="CQ61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -984,7 +1044,7 @@
     <col min="1" max="109" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1295,7 +1355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44173.674423657409</v>
       </c>
@@ -1330,7 +1390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44173.675011909727</v>
       </c>
@@ -1365,7 +1425,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44173.82585306713</v>
       </c>
@@ -1400,7 +1460,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44173.830067662042</v>
       </c>
@@ -1441,7 +1501,7 @@
         <v>26.84</v>
       </c>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44173.971974351851</v>
       </c>
@@ -1464,7 +1524,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44174.491630173608</v>
       </c>
@@ -1499,7 +1559,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44174.707013460647</v>
       </c>
@@ -1534,7 +1594,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44175.402996493052</v>
       </c>
@@ -1557,7 +1617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44175.518497777783</v>
       </c>
@@ -1601,7 +1661,7 @@
         <v>24.14</v>
       </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44175.602179386573</v>
       </c>
@@ -1639,7 +1699,7 @@
         <v>20.09</v>
       </c>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44175.625549710647</v>
       </c>
@@ -1677,7 +1737,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44175.627376412041</v>
       </c>
@@ -1715,7 +1775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44175.694606516205</v>
       </c>
@@ -1756,7 +1816,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44175.704930567124</v>
       </c>
@@ -1797,7 +1857,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44176.619537199076</v>
       </c>
@@ -1820,7 +1880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44176.700250381946</v>
       </c>
@@ -1861,7 +1921,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44176.727394224537</v>
       </c>
@@ -1902,7 +1962,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44177.436439351848</v>
       </c>
@@ -1943,7 +2003,7 @@
         <v>16.739999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44177.63497694445</v>
       </c>
@@ -1981,7 +2041,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44177.636131064814</v>
       </c>
@@ -2022,7 +2082,7 @@
         <v>15.49</v>
       </c>
     </row>
-    <row r="22" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44177.637430173607</v>
       </c>
@@ -2063,7 +2123,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44177.638555729165</v>
       </c>
@@ -2107,7 +2167,7 @@
         <v>11.29</v>
       </c>
     </row>
-    <row r="24" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44177.894269131946</v>
       </c>
@@ -2148,7 +2208,7 @@
         <v>29.27</v>
       </c>
     </row>
-    <row r="25" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44177.895198391205</v>
       </c>
@@ -2189,7 +2249,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="26" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44177.896178229166</v>
       </c>
@@ -2230,7 +2290,7 @@
         <v>12.03</v>
       </c>
     </row>
-    <row r="27" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44177.897103379626</v>
       </c>
@@ -2271,7 +2331,7 @@
         <v>21.47</v>
       </c>
     </row>
-    <row r="28" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44178.435599699078</v>
       </c>
@@ -2312,7 +2372,7 @@
         <v>31.54</v>
       </c>
     </row>
-    <row r="29" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44178.629134722221</v>
       </c>
@@ -2332,7 +2392,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44178.631708182875</v>
       </c>
@@ -2370,7 +2430,7 @@
         <v>16.329999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44178.720764652782</v>
       </c>
@@ -2402,7 +2462,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44178.721159027773</v>
       </c>
@@ -2434,7 +2494,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44178.820782233801</v>
       </c>
@@ -2469,7 +2529,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44179.081943854166</v>
       </c>
@@ -2507,7 +2567,7 @@
         <v>9.41</v>
       </c>
     </row>
-    <row r="35" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44179.095573032406</v>
       </c>
@@ -2548,7 +2608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44179.096957361107</v>
       </c>
@@ -2589,7 +2649,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="37" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44179.098243622684</v>
       </c>
@@ -2630,7 +2690,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="38" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44179.099433831019</v>
       </c>
@@ -2671,7 +2731,7 @@
         <v>12.87</v>
       </c>
     </row>
-    <row r="39" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44179.100757870372</v>
       </c>
@@ -2712,7 +2772,7 @@
         <v>15.74</v>
       </c>
     </row>
-    <row r="40" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44179.101968356481</v>
       </c>
@@ -2753,7 +2813,7 @@
         <v>6.47</v>
       </c>
     </row>
-    <row r="41" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44179.103801412042</v>
       </c>
@@ -2791,7 +2851,7 @@
         <v>15.14</v>
       </c>
     </row>
-    <row r="42" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44179.104443472221</v>
       </c>
@@ -2832,7 +2892,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="43" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44179.105701469904</v>
       </c>
@@ -2873,7 +2933,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44179.107180636573</v>
       </c>
@@ -2914,7 +2974,7 @@
         <v>57.87</v>
       </c>
     </row>
-    <row r="45" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44179.108474895838</v>
       </c>
@@ -2955,7 +3015,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44179.109649895836</v>
       </c>
@@ -2990,7 +3050,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44179.110669988426</v>
       </c>
@@ -3025,7 +3085,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44179.119340983802</v>
       </c>
@@ -3063,7 +3123,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="49" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44179.146234942134</v>
       </c>
@@ -3104,7 +3164,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="50" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44179.147582384263</v>
       </c>
@@ -3145,7 +3205,7 @@
         <v>11.12</v>
       </c>
     </row>
-    <row r="51" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44179.149365636578</v>
       </c>
@@ -3186,7 +3246,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="52" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44179.152569791666</v>
       </c>
@@ -3227,7 +3287,7 @@
         <v>24.86</v>
       </c>
     </row>
-    <row r="53" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44179.154742268518</v>
       </c>
@@ -3268,7 +3328,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44179.58322104167</v>
       </c>
@@ -3309,7 +3369,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44179.603693518518</v>
       </c>
@@ -3332,7 +3392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44179.688475104165</v>
       </c>
@@ -3355,7 +3415,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44179.690891469909</v>
       </c>
@@ -3393,7 +3453,7 @@
         <v>35.020000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44179.834601377312</v>
       </c>
@@ -3434,7 +3494,7 @@
         <v>11.96</v>
       </c>
     </row>
-    <row r="59" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44179.835298171296</v>
       </c>
@@ -3475,7 +3535,7 @@
         <v>28.58</v>
       </c>
     </row>
-    <row r="60" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:109" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44179.921338437503</v>
       </c>
@@ -3509,6 +3569,276 @@
       <c r="CO60" s="3" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="61" spans="1:109" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="8"/>
+      <c r="T61" s="8"/>
+      <c r="U61" s="8"/>
+      <c r="V61" s="8"/>
+      <c r="W61" s="8"/>
+      <c r="X61" s="8"/>
+      <c r="Y61" s="8"/>
+      <c r="Z61" s="8"/>
+      <c r="AA61" s="8"/>
+      <c r="AB61" s="8"/>
+      <c r="AC61" s="8"/>
+      <c r="AD61" s="8"/>
+      <c r="AE61" s="8"/>
+      <c r="AF61" s="8"/>
+      <c r="AG61" s="8"/>
+      <c r="AH61" s="8"/>
+      <c r="AI61" s="8"/>
+      <c r="AJ61" s="8"/>
+      <c r="AK61" s="8"/>
+      <c r="AL61" s="8"/>
+      <c r="AM61" s="8"/>
+      <c r="AN61" s="8"/>
+      <c r="AO61" s="8"/>
+      <c r="AP61" s="8"/>
+      <c r="AQ61" s="8"/>
+      <c r="AR61" s="8"/>
+      <c r="AS61" s="8"/>
+      <c r="AT61" s="8"/>
+      <c r="AU61" s="8"/>
+      <c r="AV61" s="8"/>
+      <c r="AW61" s="8"/>
+      <c r="AX61" s="8"/>
+      <c r="AY61" s="8"/>
+      <c r="AZ61" s="8"/>
+      <c r="BA61" s="8"/>
+      <c r="BB61" s="8"/>
+      <c r="BC61" s="8"/>
+      <c r="BD61" s="8"/>
+      <c r="BE61" s="8"/>
+      <c r="BF61" s="8"/>
+      <c r="BG61" s="8"/>
+      <c r="BH61" s="8"/>
+      <c r="BI61" s="8"/>
+      <c r="BJ61" s="8"/>
+      <c r="BK61" s="8"/>
+      <c r="BL61" s="8"/>
+      <c r="BM61" s="8"/>
+      <c r="BN61" s="8"/>
+      <c r="BO61" s="8"/>
+      <c r="BP61" s="8"/>
+      <c r="BQ61" s="8"/>
+      <c r="BR61" s="8"/>
+      <c r="BS61" s="8"/>
+      <c r="BT61" s="8"/>
+      <c r="BU61" s="8"/>
+      <c r="BV61" s="8"/>
+      <c r="BW61" s="8"/>
+      <c r="BX61" s="8"/>
+      <c r="BY61" s="8"/>
+      <c r="BZ61" s="8"/>
+      <c r="CA61" s="8"/>
+      <c r="CB61" s="8"/>
+      <c r="CC61" s="8"/>
+      <c r="CD61" s="8"/>
+      <c r="CE61" s="8"/>
+      <c r="CF61" s="8"/>
+      <c r="CG61" s="8"/>
+      <c r="CH61" s="8"/>
+      <c r="CI61" s="8"/>
+      <c r="CJ61" s="8"/>
+      <c r="CK61" s="8"/>
+      <c r="CL61" s="8"/>
+      <c r="CM61" s="8"/>
+      <c r="CN61" s="8"/>
+      <c r="CO61" s="8"/>
+      <c r="CP61" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="CQ61" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="CR61" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="CS61" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="CT61" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="CU61" s="8"/>
+      <c r="CV61" s="8"/>
+      <c r="CW61" s="8"/>
+      <c r="CX61" s="8"/>
+      <c r="CY61" s="8"/>
+      <c r="CZ61" s="8"/>
+      <c r="DA61" s="8"/>
+      <c r="DB61" s="8"/>
+      <c r="DC61" s="8"/>
+      <c r="DD61" s="8"/>
+      <c r="DE61" s="8"/>
+    </row>
+    <row r="62" spans="1:109" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="7">
+        <v>15.72</v>
+      </c>
+      <c r="P62" s="7">
+        <v>17.260000000000002</v>
+      </c>
+      <c r="Q62" s="7">
+        <v>32.33</v>
+      </c>
+      <c r="R62" s="7">
+        <v>27.07</v>
+      </c>
+      <c r="S62" s="7">
+        <v>19.02</v>
+      </c>
+      <c r="T62" s="7">
+        <v>15.72</v>
+      </c>
+      <c r="U62" s="7">
+        <v>21.12</v>
+      </c>
+      <c r="V62" s="8"/>
+      <c r="W62" s="8"/>
+      <c r="X62" s="8"/>
+      <c r="Y62" s="8"/>
+      <c r="Z62" s="8"/>
+      <c r="AA62" s="8"/>
+      <c r="AB62" s="8"/>
+      <c r="AC62" s="8"/>
+      <c r="AD62" s="8"/>
+      <c r="AE62" s="8"/>
+      <c r="AF62" s="8"/>
+      <c r="AG62" s="8"/>
+      <c r="AH62" s="8"/>
+      <c r="AI62" s="8"/>
+      <c r="AJ62" s="8"/>
+      <c r="AK62" s="8"/>
+      <c r="AL62" s="8"/>
+      <c r="AM62" s="8"/>
+      <c r="AN62" s="8"/>
+      <c r="AO62" s="8"/>
+      <c r="AP62" s="8"/>
+      <c r="AQ62" s="8"/>
+      <c r="AR62" s="8"/>
+      <c r="AS62" s="8"/>
+      <c r="AT62" s="8"/>
+      <c r="AU62" s="8"/>
+      <c r="AV62" s="8"/>
+      <c r="AW62" s="8"/>
+      <c r="AX62" s="8"/>
+      <c r="AY62" s="8"/>
+      <c r="AZ62" s="8"/>
+      <c r="BA62" s="8"/>
+      <c r="BB62" s="8"/>
+      <c r="BC62" s="8"/>
+      <c r="BD62" s="8"/>
+      <c r="BE62" s="8"/>
+      <c r="BF62" s="8"/>
+      <c r="BG62" s="8"/>
+      <c r="BH62" s="8"/>
+      <c r="BI62" s="8"/>
+      <c r="BJ62" s="8"/>
+      <c r="BK62" s="8"/>
+      <c r="BL62" s="8"/>
+      <c r="BM62" s="8"/>
+      <c r="BN62" s="8"/>
+      <c r="BO62" s="8"/>
+      <c r="BP62" s="8"/>
+      <c r="BQ62" s="8"/>
+      <c r="BR62" s="8"/>
+      <c r="BS62" s="8"/>
+      <c r="BT62" s="8"/>
+      <c r="BU62" s="8"/>
+      <c r="BV62" s="8"/>
+      <c r="BW62" s="8"/>
+      <c r="BX62" s="8"/>
+      <c r="BY62" s="8"/>
+      <c r="BZ62" s="8"/>
+      <c r="CA62" s="8"/>
+      <c r="CB62" s="8"/>
+      <c r="CC62" s="8"/>
+      <c r="CD62" s="8"/>
+      <c r="CE62" s="8"/>
+      <c r="CF62" s="8"/>
+      <c r="CG62" s="8"/>
+      <c r="CH62" s="8"/>
+      <c r="CI62" s="8"/>
+      <c r="CJ62" s="8"/>
+      <c r="CK62" s="8"/>
+      <c r="CL62" s="8"/>
+      <c r="CM62" s="8"/>
+      <c r="CN62" s="8"/>
+      <c r="CO62" s="8"/>
+      <c r="CP62" s="8"/>
+      <c r="CQ62" s="8"/>
+      <c r="CR62" s="8"/>
+      <c r="CS62" s="8"/>
+      <c r="CT62" s="8"/>
+      <c r="CU62" s="8"/>
+      <c r="CV62" s="8"/>
+      <c r="CW62" s="8"/>
+      <c r="CX62" s="8"/>
+      <c r="CY62" s="8"/>
+      <c r="CZ62" s="8"/>
+      <c r="DA62" s="8"/>
+      <c r="DB62" s="8"/>
+      <c r="DC62" s="8"/>
+      <c r="DD62" s="8"/>
+      <c r="DE62" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:CY60" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -3572,7 +3902,10 @@
     <hyperlink ref="F58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="F59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
     <hyperlink ref="F60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F61" r:id="rId60" xr:uid="{58457CA9-0D6D-4819-BC05-AC0B82AEACE6}"/>
+    <hyperlink ref="F62" r:id="rId61" display="https://www.facebook.com/events/1026387727837469/?post_id=1029478957528346&amp;view=permalink&amp;__cft__%5b0%5d=AZXj2U_KvS9ECavsicJ2QyUQQNeQLZCEfAxZqQ2IdscdkkcrlBiqMHiL1jf4AFfZzaXEqS_6gRy03fBEGTb5mxPmalUnU0PL7vTnFR7AdvByWLhZMm_j67ReyiQt44y1l0k&amp;__tn__=%2CO%2CP-R" xr:uid="{779B53B6-DE52-4FF1-A6AE-EF5D525BC211}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId62"/>
 </worksheet>
 </file>
</xml_diff>